<commit_message>
add prepare functions for writing
</commit_message>
<xml_diff>
--- a/rd_connect_auto.xlsx
+++ b/rd_connect_auto.xlsx
@@ -10,14 +10,15 @@
     <sheet name="packages" sheetId="1" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" r:id="rId3"/>
-    <sheet name="rd_connect_test_dir" sheetId="4" r:id="rId4"/>
+    <sheet name="rd_connect_test_directories" sheetId="4" r:id="rId4"/>
+    <sheet name="rd_connect_test_deseases" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="831">
   <si>
     <t>name</t>
   </si>
@@ -55,7 +56,7 @@
     <t>description-en</t>
   </si>
   <si>
-    <t>dir</t>
+    <t>directories</t>
   </si>
   <si>
     <t>Directory</t>
@@ -64,6 +65,9 @@
     <t>PostgreSQL</t>
   </si>
   <si>
+    <t>deseases</t>
+  </si>
+  <si>
     <t>entity</t>
   </si>
   <si>
@@ -89,9 +93,6 @@
   </si>
   <si>
     <t>date_of_inclusion</t>
-  </si>
-  <si>
-    <t>rd_connect_test_dir</t>
   </si>
   <si>
     <t>string</t>
@@ -2892,7 +2893,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2941,6 +2942,20 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2968,28 +2983,28 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -3000,13 +3015,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -3029,7 +3044,7 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -3052,7 +3067,7 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -3075,7 +3090,7 @@
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -3098,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
@@ -3121,7 +3136,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -3151,7 +3166,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
@@ -11532,4 +11547,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working import in molgenis
</commit_message>
<xml_diff>
--- a/rd_connect_auto.xlsx
+++ b/rd_connect_auto.xlsx
@@ -11,14 +11,13 @@
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" r:id="rId3"/>
     <sheet name="rd_connect_test_directories" sheetId="4" r:id="rId4"/>
-    <sheet name="rd_connect_test_deseases" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="831">
   <si>
     <t>name</t>
   </si>
@@ -65,9 +64,6 @@
     <t>PostgreSQL</t>
   </si>
   <si>
-    <t>deseases</t>
-  </si>
-  <si>
     <t>entity</t>
   </si>
   <si>
@@ -93,6 +89,9 @@
   </si>
   <si>
     <t>date_of_inclusion</t>
+  </si>
+  <si>
+    <t>rd_connect_test_directories</t>
   </si>
   <si>
     <t>string</t>
@@ -2893,7 +2892,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2942,20 +2941,6 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2983,28 +2968,28 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -3015,13 +3000,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -3044,7 +3029,7 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -3067,7 +3052,7 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -3090,7 +3075,7 @@
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -3113,7 +3098,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
@@ -3136,7 +3121,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -3166,7 +3151,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
@@ -11547,16 +11532,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
rd-connect in  emx format done
</commit_message>
<xml_diff>
--- a/rd_connect_auto.xlsx
+++ b/rd_connect_auto.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="1759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3007" uniqueCount="1759">
   <si>
     <t>name</t>
   </si>
@@ -462,10 +462,10 @@
     <t>Other4838</t>
   </si>
   <si>
+    <t>rd_bb_contribution</t>
+  </si>
+  <si>
     <t>Is_your_entire_sample_collection_available_for_the_RD-Connect_Catalogue</t>
-  </si>
-  <si>
-    <t>rd_bb_contribution</t>
   </si>
   <si>
     <t>If_not__please_specify_what_type_of_collections_can_be_publicly_available</t>
@@ -6188,7 +6188,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M152"/>
+  <dimension ref="A1:M153"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8152,7 +8152,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:10">
       <c r="A113" t="s">
         <v>138</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:10">
       <c r="A114" t="s">
         <v>139</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:10">
       <c r="A115" t="s">
         <v>140</v>
       </c>
@@ -8203,7 +8203,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:10">
       <c r="A116" t="s">
         <v>141</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:10">
       <c r="A117" t="s">
         <v>142</v>
       </c>
@@ -8237,7 +8237,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:10">
       <c r="A118" t="s">
         <v>143</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:10">
       <c r="A119" t="s">
         <v>85</v>
       </c>
@@ -8271,154 +8271,157 @@
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:10">
       <c r="A120" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
       <c r="B120" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
       <c r="C120" t="s">
         <v>35</v>
       </c>
       <c r="D120" t="s">
+        <v>144</v>
+      </c>
+      <c r="H120" t="s">
+        <v>43</v>
+      </c>
+      <c r="J120" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" t="s">
         <v>145</v>
       </c>
-      <c r="H120" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8">
-      <c r="A121" t="s">
-        <v>146</v>
-      </c>
       <c r="B121" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C121" t="s">
         <v>35</v>
       </c>
       <c r="D121" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H121" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:10">
       <c r="A122" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B122" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C122" t="s">
         <v>35</v>
       </c>
       <c r="D122" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H122" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:10">
       <c r="A123" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B123" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C123" t="s">
         <v>35</v>
       </c>
       <c r="D123" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H123" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:10">
       <c r="A124" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B124" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C124" t="s">
         <v>35</v>
       </c>
       <c r="D124" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H124" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:10">
       <c r="A125" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B125" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C125" t="s">
         <v>35</v>
       </c>
       <c r="D125" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H125" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:10">
       <c r="A126" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B126" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C126" t="s">
         <v>35</v>
       </c>
       <c r="D126" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H126" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:10">
       <c r="A127" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B127" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C127" t="s">
         <v>35</v>
       </c>
       <c r="D127" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H127" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:10">
       <c r="A128" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B128" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C128" t="s">
         <v>35</v>
       </c>
       <c r="D128" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H128" t="s">
         <v>37</v>
@@ -8426,16 +8429,16 @@
     </row>
     <row r="129" spans="1:10">
       <c r="A129" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="B129" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="C129" t="s">
         <v>35</v>
       </c>
       <c r="D129" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H129" t="s">
         <v>37</v>
@@ -8443,30 +8446,27 @@
     </row>
     <row r="130" spans="1:10">
       <c r="A130" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B130" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C130" t="s">
         <v>35</v>
       </c>
       <c r="D130" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="H130" t="s">
-        <v>43</v>
-      </c>
-      <c r="J130" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="131" spans="1:10">
       <c r="A131" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="B131" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="C131" t="s">
         <v>35</v>
@@ -8475,15 +8475,18 @@
         <v>154</v>
       </c>
       <c r="H131" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="J131" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="132" spans="1:10">
       <c r="A132" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B132" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C132" t="s">
         <v>35</v>
@@ -8497,10 +8500,10 @@
     </row>
     <row r="133" spans="1:10">
       <c r="A133" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="B133" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="C133" t="s">
         <v>35</v>
@@ -8514,10 +8517,10 @@
     </row>
     <row r="134" spans="1:10">
       <c r="A134" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="B134" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="C134" t="s">
         <v>35</v>
@@ -8531,10 +8534,10 @@
     </row>
     <row r="135" spans="1:10">
       <c r="A135" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="B135" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="C135" t="s">
         <v>35</v>
@@ -8548,10 +8551,10 @@
     </row>
     <row r="136" spans="1:10">
       <c r="A136" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="B136" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="C136" t="s">
         <v>35</v>
@@ -8565,10 +8568,10 @@
     </row>
     <row r="137" spans="1:10">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B137" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C137" t="s">
         <v>35</v>
@@ -8582,10 +8585,10 @@
     </row>
     <row r="138" spans="1:10">
       <c r="A138" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B138" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="C138" t="s">
         <v>35</v>
@@ -8599,10 +8602,10 @@
     </row>
     <row r="139" spans="1:10">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="B139" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C139" t="s">
         <v>35</v>
@@ -8616,10 +8619,10 @@
     </row>
     <row r="140" spans="1:10">
       <c r="A140" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B140" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="C140" t="s">
         <v>35</v>
@@ -8633,10 +8636,10 @@
     </row>
     <row r="141" spans="1:10">
       <c r="A141" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="B141" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="C141" t="s">
         <v>35</v>
@@ -8650,10 +8653,10 @@
     </row>
     <row r="142" spans="1:10">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B142" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C142" t="s">
         <v>35</v>
@@ -8667,10 +8670,10 @@
     </row>
     <row r="143" spans="1:10">
       <c r="A143" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B143" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C143" t="s">
         <v>35</v>
@@ -8684,10 +8687,10 @@
     </row>
     <row r="144" spans="1:10">
       <c r="A144" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="C144" t="s">
         <v>35</v>
@@ -8701,30 +8704,27 @@
     </row>
     <row r="145" spans="1:10">
       <c r="A145" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B145" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C145" t="s">
         <v>35</v>
       </c>
       <c r="D145" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H145" t="s">
-        <v>43</v>
-      </c>
-      <c r="J145" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="146" spans="1:10">
       <c r="A146" t="s">
-        <v>160</v>
+        <v>42</v>
       </c>
       <c r="B146" t="s">
-        <v>160</v>
+        <v>42</v>
       </c>
       <c r="C146" t="s">
         <v>35</v>
@@ -8733,15 +8733,18 @@
         <v>159</v>
       </c>
       <c r="H146" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="J146" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="147" spans="1:10">
       <c r="A147" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B147" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C147" t="s">
         <v>35</v>
@@ -8755,10 +8758,10 @@
     </row>
     <row r="148" spans="1:10">
       <c r="A148" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B148" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C148" t="s">
         <v>35</v>
@@ -8772,10 +8775,10 @@
     </row>
     <row r="149" spans="1:10">
       <c r="A149" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B149" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C149" t="s">
         <v>35</v>
@@ -8789,10 +8792,10 @@
     </row>
     <row r="150" spans="1:10">
       <c r="A150" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B150" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C150" t="s">
         <v>35</v>
@@ -8806,10 +8809,10 @@
     </row>
     <row r="151" spans="1:10">
       <c r="A151" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B151" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C151" t="s">
         <v>35</v>
@@ -8823,10 +8826,10 @@
     </row>
     <row r="152" spans="1:10">
       <c r="A152" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="B152" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="C152" t="s">
         <v>35</v>
@@ -8835,6 +8838,23 @@
         <v>159</v>
       </c>
       <c r="H152" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
+      <c r="A153" t="s">
+        <v>85</v>
+      </c>
+      <c r="B153" t="s">
+        <v>85</v>
+      </c>
+      <c r="C153" t="s">
+        <v>35</v>
+      </c>
+      <c r="D153" t="s">
+        <v>159</v>
+      </c>
+      <c r="H153" t="s">
         <v>37</v>
       </c>
     </row>
@@ -17436,41 +17456,44 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
         <v>146</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>147</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>148</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>149</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>150</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>151</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>152</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>153</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>